<commit_message>
implemented first working function and samples generating valid GTFS feed
</commit_message>
<xml_diff>
--- a/samples/simplexl/Albtal_H.xlsx
+++ b/samples/simplexl/Albtal_H.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\VisualStudioCode\x2gtfs\samples\simplexl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C7FC90-8773-484B-AD00-8D2655862DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C25E1A-2896-4199-89D7-DC7AEB8F26DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3765" windowWidth="38640" windowHeight="21120" xr2:uid="{F9DF9B2E-BC96-47A3-9FE7-DCF8D64A86E8}"/>
+    <workbookView xWindow="67080" yWindow="-3645" windowWidth="38640" windowHeight="21120" xr2:uid="{F9DF9B2E-BC96-47A3-9FE7-DCF8D64A86E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
     <t>A5</t>
   </si>
   <si>
-    <t>BfFestAlbtal</t>
+    <t>BahnhofsfestAlbtal</t>
   </si>
 </sst>
 </file>
@@ -509,7 +509,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>